<commit_message>
Transport cover sheet updated
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35B45B9-E7F2-4FD4-B19F-B29F203A353C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21C8F2E-7974-408D-B30C-BB949057CED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" tabRatio="909" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="47" r:id="rId1"/>
@@ -19,7 +19,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -142,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>IE</t>
   </si>
@@ -371,27 +370,15 @@
     <t>Document type:</t>
   </si>
   <si>
-    <t>Template type</t>
-  </si>
-  <si>
     <t>Sector(s):</t>
   </si>
   <si>
-    <t>Sector name</t>
-  </si>
-  <si>
     <t>Purpose:</t>
   </si>
   <si>
-    <t>Brief description of what this file is for</t>
-  </si>
-  <si>
     <t>Original developer(s):</t>
   </si>
   <si>
-    <t>Full Name(s) (Affiliation, email)</t>
-  </si>
-  <si>
     <t>Current maintainer(s):</t>
   </si>
   <si>
@@ -411,6 +398,21 @@
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>New Technology</t>
+  </si>
+  <si>
+    <t>Transport (TRA)</t>
+  </si>
+  <si>
+    <t>Vahid Aryanpur (UCC, vahid.aryanpur@ucc.ie)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olexandr Balyk ( MaREI, olexandr.balyk@ucc.ie) </t>
+  </si>
+  <si>
+    <t>Assign new vehicle data</t>
   </si>
 </sst>
 </file>
@@ -696,9 +698,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -717,9 +716,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -732,14 +728,20 @@
     <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1090,7 +1092,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1102,7 +1104,7 @@
                   <a14:compatExt spid="_x0000_s89089"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000015C0100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000015C0100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1270,19 +1272,6 @@
       <sheetData sheetId="56"/>
       <sheetData sheetId="57"/>
       <sheetData sheetId="58"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1612,25 +1601,25 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" style="16" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="16" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="16" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="16" customWidth="1"/>
+    <col min="1" max="4" width="21.6640625" style="16" customWidth="1"/>
+    <col min="5" max="6" width="14.109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="16" customWidth="1"/>
+    <col min="8" max="10" width="8.109375" style="16" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" style="16" customWidth="1"/>
     <col min="13" max="13" width="10" style="16" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="16" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="16"/>
+    <col min="14" max="14" width="11.44140625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" style="16" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1658,7 +1647,7 @@
       <c r="Y1" s="15"/>
       <c r="Z1" s="15"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1686,7 +1675,7 @@
       <c r="Y2" s="15"/>
       <c r="Z2" s="15"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -1714,7 +1703,7 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -1742,7 +1731,7 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -1770,7 +1759,7 @@
       <c r="Y5" s="15"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -1798,7 +1787,7 @@
       <c r="Y6" s="15"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1826,7 +1815,7 @@
       <c r="Y7" s="15"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1854,7 +1843,7 @@
       <c r="Y8" s="15"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -1882,7 +1871,7 @@
       <c r="Y9" s="15"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1910,7 +1899,7 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -1938,7 +1927,7 @@
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -1966,7 +1955,7 @@
       <c r="Y12" s="15"/>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -1994,7 +1983,7 @@
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -2022,7 +2011,7 @@
       <c r="Y14" s="15"/>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -2050,21 +2039,21 @@
       <c r="Y15" s="15"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
@@ -2080,11 +2069,11 @@
       <c r="Y16" s="15"/>
       <c r="Z16" s="15"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -2108,19 +2097,19 @@
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
@@ -2136,23 +2125,23 @@
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
+      <c r="B19" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
@@ -2168,23 +2157,23 @@
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
@@ -2200,23 +2189,23 @@
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
@@ -2232,19 +2221,19 @@
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
@@ -2260,15 +2249,15 @@
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -2292,11 +2281,11 @@
       <c r="Y23" s="15"/>
       <c r="Z23" s="15"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -2320,11 +2309,11 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -2348,15 +2337,15 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -2380,11 +2369,13 @@
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -2408,11 +2399,11 @@
       <c r="Y27" s="15"/>
       <c r="Z27" s="15"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -2436,15 +2427,15 @@
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="28">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="26">
         <v>1</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -2468,17 +2459,17 @@
       <c r="Y29" s="15"/>
       <c r="Z29" s="15"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
@@ -2500,17 +2491,17 @@
       <c r="Y30" s="15"/>
       <c r="Z30" s="15"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
@@ -2532,13 +2523,13 @@
       <c r="Y31" s="15"/>
       <c r="Z31" s="15"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
@@ -2562,7 +2553,7 @@
       <c r="Y32" s="15"/>
       <c r="Z32" s="15"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -2590,7 +2581,7 @@
       <c r="Y33" s="15"/>
       <c r="Z33" s="15"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -2618,7 +2609,7 @@
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -2646,7 +2637,7 @@
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -2674,7 +2665,7 @@
       <c r="Y36" s="15"/>
       <c r="Z36" s="15"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -2702,7 +2693,7 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2730,7 +2721,7 @@
       <c r="Y38" s="15"/>
       <c r="Z38" s="15"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -2758,7 +2749,7 @@
       <c r="Y39" s="15"/>
       <c r="Z39" s="15"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -2786,7 +2777,7 @@
       <c r="Y40" s="15"/>
       <c r="Z40" s="15"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -2814,7 +2805,7 @@
       <c r="Y41" s="15"/>
       <c r="Z41" s="15"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -2842,7 +2833,7 @@
       <c r="Y42" s="15"/>
       <c r="Z42" s="15"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -2870,7 +2861,7 @@
       <c r="Y43" s="15"/>
       <c r="Z43" s="15"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -2898,7 +2889,7 @@
       <c r="Y44" s="15"/>
       <c r="Z44" s="15"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -2926,7 +2917,7 @@
       <c r="Y45" s="15"/>
       <c r="Z45" s="15"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -2954,7 +2945,7 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -2982,7 +2973,7 @@
       <c r="Y47" s="15"/>
       <c r="Z47" s="15"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -3010,7 +3001,7 @@
       <c r="Y48" s="15"/>
       <c r="Z48" s="15"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -3038,7 +3029,7 @@
       <c r="Y49" s="15"/>
       <c r="Z49" s="15"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -3066,7 +3057,7 @@
       <c r="Y50" s="15"/>
       <c r="Z50" s="15"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
@@ -3094,7 +3085,7 @@
       <c r="Y51" s="15"/>
       <c r="Z51" s="15"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -3122,7 +3113,7 @@
       <c r="Y52" s="15"/>
       <c r="Z52" s="15"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -3150,7 +3141,7 @@
       <c r="Y53" s="15"/>
       <c r="Z53" s="15"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
@@ -3178,7 +3169,7 @@
       <c r="Y54" s="15"/>
       <c r="Z54" s="15"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
@@ -3206,7 +3197,7 @@
       <c r="Y55" s="15"/>
       <c r="Z55" s="15"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
@@ -3234,7 +3225,7 @@
       <c r="Y56" s="15"/>
       <c r="Z56" s="15"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
@@ -3262,7 +3253,7 @@
       <c r="Y57" s="15"/>
       <c r="Z57" s="15"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
@@ -3290,7 +3281,7 @@
       <c r="Y58" s="15"/>
       <c r="Z58" s="15"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
@@ -3318,7 +3309,7 @@
       <c r="Y59" s="15"/>
       <c r="Z59" s="15"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="15"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
@@ -3346,7 +3337,7 @@
       <c r="Y60" s="15"/>
       <c r="Z60" s="15"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="15"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
@@ -3374,7 +3365,7 @@
       <c r="Y61" s="15"/>
       <c r="Z61" s="15"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="15"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
@@ -3402,7 +3393,7 @@
       <c r="Y62" s="15"/>
       <c r="Z62" s="15"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
@@ -3430,7 +3421,7 @@
       <c r="Y63" s="15"/>
       <c r="Z63" s="15"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -3458,7 +3449,7 @@
       <c r="Y64" s="15"/>
       <c r="Z64" s="15"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
@@ -3486,7 +3477,7 @@
       <c r="Y65" s="15"/>
       <c r="Z65" s="15"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
@@ -3514,7 +3505,7 @@
       <c r="Y66" s="15"/>
       <c r="Z66" s="15"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
@@ -3542,7 +3533,7 @@
       <c r="Y67" s="15"/>
       <c r="Z67" s="15"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
@@ -3570,7 +3561,7 @@
       <c r="Y68" s="15"/>
       <c r="Z68" s="15"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="15"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
@@ -3598,7 +3589,7 @@
       <c r="Y69" s="15"/>
       <c r="Z69" s="15"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="15"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
@@ -3626,7 +3617,7 @@
       <c r="Y70" s="15"/>
       <c r="Z70" s="15"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
@@ -3654,7 +3645,7 @@
       <c r="Y71" s="15"/>
       <c r="Z71" s="15"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="15"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
@@ -3682,7 +3673,7 @@
       <c r="Y72" s="15"/>
       <c r="Z72" s="15"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
@@ -3710,7 +3701,7 @@
       <c r="Y73" s="15"/>
       <c r="Z73" s="15"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="15"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
@@ -3738,7 +3729,7 @@
       <c r="Y74" s="15"/>
       <c r="Z74" s="15"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="15"/>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>
@@ -3766,7 +3757,7 @@
       <c r="Y75" s="15"/>
       <c r="Z75" s="15"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="15"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
@@ -3794,7 +3785,7 @@
       <c r="Y76" s="15"/>
       <c r="Z76" s="15"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="15"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
@@ -3822,7 +3813,7 @@
       <c r="Y77" s="15"/>
       <c r="Z77" s="15"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="15"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
@@ -3850,7 +3841,7 @@
       <c r="Y78" s="15"/>
       <c r="Z78" s="15"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="15"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
@@ -3878,7 +3869,7 @@
       <c r="Y79" s="15"/>
       <c r="Z79" s="15"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="15"/>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
@@ -3906,7 +3897,7 @@
       <c r="Y80" s="15"/>
       <c r="Z80" s="15"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="15"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
@@ -3934,7 +3925,7 @@
       <c r="Y81" s="15"/>
       <c r="Z81" s="15"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="15"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
@@ -3962,7 +3953,7 @@
       <c r="Y82" s="15"/>
       <c r="Z82" s="15"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="15"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
@@ -3990,7 +3981,7 @@
       <c r="Y83" s="15"/>
       <c r="Z83" s="15"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="15"/>
       <c r="B84" s="15"/>
       <c r="C84" s="15"/>
@@ -4018,7 +4009,7 @@
       <c r="Y84" s="15"/>
       <c r="Z84" s="15"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="15"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
@@ -4046,7 +4037,7 @@
       <c r="Y85" s="15"/>
       <c r="Z85" s="15"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="15"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
@@ -4074,7 +4065,7 @@
       <c r="Y86" s="15"/>
       <c r="Z86" s="15"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87" s="15"/>
       <c r="B87" s="15"/>
       <c r="C87" s="15"/>
@@ -4102,7 +4093,7 @@
       <c r="Y87" s="15"/>
       <c r="Z87" s="15"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" s="15"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
@@ -4130,7 +4121,7 @@
       <c r="Y88" s="15"/>
       <c r="Z88" s="15"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="15"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
@@ -4158,7 +4149,7 @@
       <c r="Y89" s="15"/>
       <c r="Z89" s="15"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="15"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
@@ -4186,7 +4177,7 @@
       <c r="Y90" s="15"/>
       <c r="Z90" s="15"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="15"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
@@ -4214,7 +4205,7 @@
       <c r="Y91" s="15"/>
       <c r="Z91" s="15"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="15"/>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
@@ -4242,7 +4233,7 @@
       <c r="Y92" s="15"/>
       <c r="Z92" s="15"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" s="15"/>
       <c r="B93" s="15"/>
       <c r="C93" s="15"/>
@@ -4270,7 +4261,7 @@
       <c r="Y93" s="15"/>
       <c r="Z93" s="15"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" s="15"/>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
@@ -4298,7 +4289,7 @@
       <c r="Y94" s="15"/>
       <c r="Z94" s="15"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" s="15"/>
       <c r="B95" s="15"/>
       <c r="C95" s="15"/>
@@ -4326,7 +4317,7 @@
       <c r="Y95" s="15"/>
       <c r="Z95" s="15"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" s="15"/>
       <c r="B96" s="15"/>
       <c r="C96" s="15"/>
@@ -4354,7 +4345,7 @@
       <c r="Y96" s="15"/>
       <c r="Z96" s="15"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A97" s="15"/>
       <c r="B97" s="15"/>
       <c r="C97" s="15"/>
@@ -4382,7 +4373,7 @@
       <c r="Y97" s="15"/>
       <c r="Z97" s="15"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A98" s="15"/>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
@@ -4410,7 +4401,7 @@
       <c r="Y98" s="15"/>
       <c r="Z98" s="15"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A99" s="15"/>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
@@ -4439,7 +4430,7 @@
       <c r="Z99" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="B19:D19"/>
@@ -4447,6 +4438,7 @@
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B27:D27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B30" r:id="rId1" xr:uid="{FCEDB3AE-7147-44D8-AACA-A71925D4CECD}"/>
@@ -4467,40 +4459,40 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="7" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" style="7" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="7"/>
+    <col min="29" max="29" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -4614,12 +4606,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -4734,7 +4726,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -4851,7 +4843,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -4968,7 +4960,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
@@ -4976,7 +4968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -4984,7 +4976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -4992,7 +4984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
@@ -5000,7 +4992,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
@@ -5008,7 +5000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>23</v>
       </c>
@@ -5016,7 +5008,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>25</v>
       </c>
@@ -5024,7 +5016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>27</v>
       </c>
@@ -5032,7 +5024,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>29</v>
       </c>
@@ -5040,7 +5032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>31</v>
       </c>
@@ -5048,7 +5040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>33</v>
       </c>
@@ -5056,7 +5048,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>35</v>
       </c>
@@ -5064,7 +5056,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>37</v>
       </c>
@@ -5072,7 +5064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>39</v>
       </c>
@@ -5080,7 +5072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>41</v>
       </c>
@@ -5088,7 +5080,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>43</v>
       </c>
@@ -5096,7 +5088,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>45</v>
       </c>
@@ -5104,7 +5096,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>47</v>
       </c>
@@ -5112,7 +5104,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>49</v>
       </c>
@@ -5120,7 +5112,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>51</v>
       </c>
@@ -5128,7 +5120,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>53</v>
       </c>
@@ -5136,7 +5128,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>55</v>
       </c>
@@ -5144,7 +5136,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>57</v>
       </c>
@@ -5152,7 +5144,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>59</v>
       </c>
@@ -5160,7 +5152,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>61</v>
       </c>
@@ -5168,7 +5160,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>63</v>
       </c>
@@ -5176,7 +5168,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>65</v>
       </c>
@@ -5184,7 +5176,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>67</v>
       </c>
@@ -5210,7 +5202,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -5234,42 +5226,42 @@
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="6" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5292,7 +5284,7 @@
       <c r="Y3"/>
       <c r="Z3"/>
     </row>
-    <row r="4" spans="2:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:34" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5420,7 +5412,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5509,7 +5501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
@@ -5529,7 +5521,7 @@
       <c r="Y6"/>
       <c r="Z6"/>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>

</xml_diff>